<commit_message>
I spent all day in PQ, so I just made a note in 134 to log that effort.
</commit_message>
<xml_diff>
--- a/CH-134 Final Week of the Month.xlsx
+++ b/CH-134 Final Week of the Month.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04D9A1A-677F-4767-A4FD-A607FC66A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F8A216-310A-456F-8CB3-C4A068527852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="12">
   <si>
     <t>Result</t>
   </si>
@@ -122,12 +122,15 @@
   <si>
     <t>This is a nice tight solution</t>
   </si>
+  <si>
+    <t>I need to apply this to a work problem.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +165,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -363,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,6 +439,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1588,7 +1599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CD64CC-29BF-4E16-BAA8-21065F0ED335}">
   <dimension ref="C1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19:I21"/>
     </sheetView>
   </sheetViews>
@@ -2340,7 +2351,7 @@
   <dimension ref="C1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2533,6 +2544,9 @@
       </c>
       <c r="I10">
         <v>91</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="3:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>